<commit_message>
Update Hilink智能家居 Profile V2.1 遥控大师_小苹果1_v1.1.xlsx
文档更新
</commit_message>
<xml_diff>
--- a/资料/设计方案/Hilink智能家居 Profile V2.1 遥控大师_小苹果1_v1.1.xlsx
+++ b/资料/设计方案/Hilink智能家居 Profile V2.1 遥控大师_小苹果1_v1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="95" windowWidth="19195" windowHeight="11642"/>
   </bookViews>
   <sheets>
     <sheet name="设备属性表" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="277">
   <si>
     <t>设备类型
 deviceType</t>
@@ -1230,20 +1230,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>power</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0-关机
 1-开机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电源按键</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1417,6 +1409,20 @@
   </si>
   <si>
     <t>遥控器设备devId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电源按键（不要用）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.为自动，抽湿时，温度设16度
+2.抽湿，风速1档
+3.送风，无自动档风</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1888,7 +1894,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2207,6 +2213,9 @@
     <xf numFmtId="176" fontId="10" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="24" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2216,8 +2225,11 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="24" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="176" fontId="10" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2527,11 +2539,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
@@ -2542,23 +2554,23 @@
     <col min="7" max="7" width="12.75" customWidth="1"/>
     <col min="8" max="8" width="16.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.125" customWidth="1"/>
-    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
     <col min="12" max="12" width="6.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.625" customWidth="1"/>
     <col min="15" max="15" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="14.25" thickBot="1">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="13.6" thickBot="1">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="108"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="109"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="N1" s="3"/>
@@ -2567,7 +2579,7 @@
       <c r="E2" s="59"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" ht="82.5">
+    <row r="3" spans="1:15" s="8" customFormat="1" ht="81.55">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="65" customFormat="1" ht="16.5">
+    <row r="4" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A4" s="63"/>
       <c r="B4" s="63"/>
       <c r="C4" s="63" t="s">
@@ -2637,7 +2649,7 @@
       <c r="N4" s="63"/>
       <c r="O4" s="19"/>
     </row>
-    <row r="5" spans="1:15" s="65" customFormat="1" ht="33">
+    <row r="5" spans="1:15" s="65" customFormat="1" ht="29.9">
       <c r="A5" s="63"/>
       <c r="B5" s="63"/>
       <c r="C5" s="63"/>
@@ -2666,11 +2678,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="65" customFormat="1" ht="16.5">
+    <row r="6" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A6" s="63"/>
       <c r="B6" s="63"/>
       <c r="C6" s="63" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D6" s="63" t="s">
         <v>193</v>
@@ -2691,7 +2703,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="65" customFormat="1" ht="16.5">
+    <row r="7" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A7" s="63"/>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -2724,20 +2736,20 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="65" customFormat="1" ht="82.5">
+    <row r="8" spans="1:15" s="65" customFormat="1" ht="74.75">
       <c r="A8" s="63"/>
       <c r="B8" s="63"/>
       <c r="C8" s="63"/>
       <c r="D8" s="63"/>
       <c r="E8" s="20"/>
       <c r="F8" s="89" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G8" s="89" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="88" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="17"/>
@@ -2746,10 +2758,10 @@
       <c r="M8" s="64"/>
       <c r="N8" s="63"/>
       <c r="O8" s="20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A9" s="63"/>
       <c r="B9" s="63"/>
       <c r="C9" s="63"/>
@@ -2772,7 +2784,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="83" customFormat="1" ht="16.5">
+    <row r="10" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A10" s="71"/>
       <c r="B10" s="71"/>
       <c r="C10" s="71"/>
@@ -2792,10 +2804,10 @@
       <c r="M10" s="77"/>
       <c r="N10" s="71"/>
       <c r="O10" s="78" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A11" s="63"/>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -2819,10 +2831,10 @@
       <c r="M11" s="64"/>
       <c r="N11" s="63"/>
       <c r="O11" s="66" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A12" s="71"/>
       <c r="B12" s="71"/>
       <c r="C12" s="71"/>
@@ -2842,10 +2854,10 @@
       <c r="M12" s="77"/>
       <c r="N12" s="71"/>
       <c r="O12" s="78" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A13" s="71"/>
       <c r="B13" s="71"/>
       <c r="C13" s="71"/>
@@ -2865,10 +2877,10 @@
       <c r="M13" s="77"/>
       <c r="N13" s="71"/>
       <c r="O13" s="78" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A14" s="71"/>
       <c r="B14" s="71"/>
       <c r="C14" s="71"/>
@@ -2890,10 +2902,10 @@
       <c r="M14" s="77"/>
       <c r="N14" s="71"/>
       <c r="O14" s="78" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A15" s="71"/>
       <c r="B15" s="71"/>
       <c r="C15" s="71"/>
@@ -2913,10 +2925,10 @@
       <c r="M15" s="77"/>
       <c r="N15" s="71"/>
       <c r="O15" s="78" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A16" s="71"/>
       <c r="B16" s="71"/>
       <c r="C16" s="71"/>
@@ -2927,7 +2939,7 @@
       </c>
       <c r="G16" s="79"/>
       <c r="H16" s="78" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I16" s="75"/>
       <c r="J16" s="76"/>
@@ -2936,10 +2948,10 @@
       <c r="M16" s="77"/>
       <c r="N16" s="71"/>
       <c r="O16" s="78" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A17" s="63"/>
       <c r="B17" s="63"/>
       <c r="C17" s="63"/>
@@ -2952,7 +2964,7 @@
         <v>81</v>
       </c>
       <c r="H17" s="66" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="20"/>
@@ -2961,7 +2973,7 @@
       <c r="M17" s="64"/>
       <c r="N17" s="63"/>
       <c r="O17" s="15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="83" customFormat="1" ht="20.25" customHeight="1">
@@ -2984,7 +2996,7 @@
       <c r="M18" s="77"/>
       <c r="N18" s="71"/>
       <c r="O18" s="81" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="65" customFormat="1" ht="20.25" customHeight="1">
@@ -3011,10 +3023,10 @@
       <c r="M19" s="64"/>
       <c r="N19" s="63"/>
       <c r="O19" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="83" customFormat="1" ht="16.5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="83" customFormat="1" ht="14.95">
       <c r="A20" s="71"/>
       <c r="B20" s="71"/>
       <c r="C20" s="71"/>
@@ -3034,7 +3046,7 @@
       <c r="M20" s="77"/>
       <c r="N20" s="71"/>
       <c r="O20" s="81" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="83" customFormat="1" ht="20.25" customHeight="1">
@@ -3059,10 +3071,10 @@
       <c r="M21" s="77"/>
       <c r="N21" s="71"/>
       <c r="O21" s="81" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A22" s="63"/>
       <c r="B22" s="63"/>
       <c r="C22" s="63"/>
@@ -3075,7 +3087,7 @@
         <v>81</v>
       </c>
       <c r="H22" s="66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="20"/>
@@ -3087,18 +3099,18 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="65" customFormat="1" ht="16.5">
+    <row r="23" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
       <c r="D23" s="63"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="109" t="s">
-        <v>274</v>
+      <c r="F23" s="106" t="s">
+        <v>272</v>
       </c>
       <c r="G23" s="95"/>
       <c r="H23" s="90" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I23" s="91"/>
       <c r="J23" s="92"/>
@@ -3107,10 +3119,10 @@
       <c r="M23" s="93"/>
       <c r="N23" s="89"/>
       <c r="O23" s="94" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
       <c r="C24" s="63" t="s">
@@ -3135,20 +3147,20 @@
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="65" customFormat="1" ht="181.5">
+    <row r="25" spans="1:15" s="65" customFormat="1" ht="164.4">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
       <c r="C25" s="63"/>
       <c r="D25" s="63"/>
       <c r="E25" s="20"/>
       <c r="F25" s="90" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G25" s="95" t="s">
         <v>81</v>
       </c>
       <c r="H25" s="90" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I25" s="91"/>
       <c r="J25" s="92"/>
@@ -3157,10 +3169,10 @@
       <c r="M25" s="93"/>
       <c r="N25" s="89"/>
       <c r="O25" s="94" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A26" s="63"/>
       <c r="B26" s="63"/>
       <c r="C26" s="96"/>
@@ -3171,7 +3183,7 @@
       </c>
       <c r="G26" s="99"/>
       <c r="H26" s="100" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I26" s="101"/>
       <c r="J26" s="102"/>
@@ -3180,10 +3192,10 @@
       <c r="M26" s="103"/>
       <c r="N26" s="96"/>
       <c r="O26" s="104" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A27" s="63"/>
       <c r="B27" s="63"/>
       <c r="C27" s="96"/>
@@ -3205,10 +3217,10 @@
       <c r="M27" s="103"/>
       <c r="N27" s="96"/>
       <c r="O27" s="104" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A28" s="63"/>
       <c r="B28" s="63"/>
       <c r="C28" s="96"/>
@@ -3230,10 +3242,10 @@
       <c r="M28" s="103"/>
       <c r="N28" s="96"/>
       <c r="O28" s="104" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="65" customFormat="1" ht="16.5">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="65" customFormat="1" ht="14.95">
       <c r="A29" s="63"/>
       <c r="B29" s="63"/>
       <c r="C29" s="63" t="s">
@@ -3258,36 +3270,36 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="65" customFormat="1" ht="33">
-      <c r="A30" s="63"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="19" t="s">
+    <row r="30" spans="1:15" s="110" customFormat="1" ht="29.9">
+      <c r="A30" s="96"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="101" t="s">
+        <v>234</v>
+      </c>
+      <c r="G30" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="97" t="s">
         <v>235</v>
       </c>
-      <c r="G30" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="65" customFormat="1" ht="82.5">
+      <c r="K30" s="103"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="103"/>
+      <c r="N30" s="96"/>
+      <c r="O30" s="104" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="65" customFormat="1" ht="74.75">
       <c r="A31" s="63"/>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -3308,7 +3320,9 @@
       <c r="J31" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="K31" s="64"/>
+      <c r="K31" s="111" t="s">
+        <v>276</v>
+      </c>
       <c r="L31" s="64"/>
       <c r="M31" s="64"/>
       <c r="N31" s="63"/>
@@ -3316,7 +3330,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="65" customFormat="1" ht="66">
+    <row r="32" spans="1:15" s="65" customFormat="1" ht="59.8">
       <c r="A32" s="63"/>
       <c r="B32" s="63"/>
       <c r="C32" s="63"/>
@@ -3337,7 +3351,7 @@
       <c r="J32" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="K32" s="64"/>
+      <c r="K32" s="111"/>
       <c r="L32" s="64"/>
       <c r="M32" s="64"/>
       <c r="N32" s="63"/>
@@ -3345,7 +3359,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="65" customFormat="1" ht="16.5">
+    <row r="33" spans="1:20" s="65" customFormat="1" ht="14.95">
       <c r="A33" s="63"/>
       <c r="B33" s="63"/>
       <c r="C33" s="63"/>
@@ -3365,7 +3379,7 @@
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="64" t="s">
-        <v>234</v>
+        <v>274</v>
       </c>
       <c r="L33" s="64" t="s">
         <v>227</v>
@@ -3378,7 +3392,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="65" customFormat="1" ht="33">
+    <row r="34" spans="1:20" s="65" customFormat="1" ht="29.9">
       <c r="A34" s="63"/>
       <c r="B34" s="63"/>
       <c r="C34" s="63"/>
@@ -3407,7 +3421,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="65" customFormat="1" ht="33">
+    <row r="35" spans="1:20" s="65" customFormat="1" ht="29.9">
       <c r="A35" s="63"/>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -3436,7 +3450,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="65" customFormat="1" ht="16.5">
+    <row r="36" spans="1:20" s="65" customFormat="1" ht="14.95">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
       <c r="C36" s="63" t="s">
@@ -3461,7 +3475,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="65" customFormat="1" ht="16.5">
+    <row r="37" spans="1:20" s="65" customFormat="1" ht="14.95">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
       <c r="C37" s="63"/>
@@ -3474,7 +3488,7 @@
         <v>81</v>
       </c>
       <c r="H37" s="66" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="20"/>
@@ -3486,20 +3500,20 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="65" customFormat="1" ht="16.5">
+    <row r="38" spans="1:20" s="65" customFormat="1" ht="14.95">
       <c r="A38" s="63"/>
       <c r="B38" s="63"/>
       <c r="C38" s="63"/>
       <c r="D38" s="63"/>
       <c r="E38" s="20"/>
       <c r="F38" s="88" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G38" s="89" t="s">
         <v>81</v>
       </c>
       <c r="H38" s="90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I38" s="91"/>
       <c r="J38" s="92"/>
@@ -3508,23 +3522,23 @@
       <c r="M38" s="93"/>
       <c r="N38" s="89"/>
       <c r="O38" s="94" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" s="65" customFormat="1" ht="16.5">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="65" customFormat="1" ht="14.95">
       <c r="A39" s="63"/>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
       <c r="D39" s="63"/>
       <c r="E39" s="20"/>
       <c r="F39" s="88" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G39" s="89" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H39" s="90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I39" s="91"/>
       <c r="J39" s="92"/>
@@ -3533,10 +3547,10 @@
       <c r="M39" s="93"/>
       <c r="N39" s="89"/>
       <c r="O39" s="94" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" s="67" customFormat="1" ht="16.5">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13" t="s">
@@ -3559,7 +3573,7 @@
       <c r="N40" s="18"/>
       <c r="O40" s="16"/>
     </row>
-    <row r="41" spans="1:20" s="67" customFormat="1" ht="116.25" customHeight="1">
+    <row r="41" spans="1:20" s="67" customFormat="1" ht="116.35" customHeight="1">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3594,7 +3608,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="67" customFormat="1" ht="16.5">
+    <row r="42" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -3623,7 +3637,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="67" customFormat="1" ht="16.5">
+    <row r="43" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3648,7 +3662,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="67" customFormat="1" ht="16.5">
+    <row r="44" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3673,7 +3687,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="67" customFormat="1" ht="16.5">
+    <row r="45" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3698,7 +3712,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="67" customFormat="1" ht="16.5">
+    <row r="46" spans="1:20" s="67" customFormat="1" ht="14.95">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13" t="s">
@@ -3723,7 +3737,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="69" customFormat="1" ht="33">
+    <row r="47" spans="1:20" s="69" customFormat="1" ht="29.9">
       <c r="A47" s="22"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -3759,7 +3773,7 @@
       <c r="S47" s="67"/>
       <c r="T47" s="67"/>
     </row>
-    <row r="48" spans="1:20" s="69" customFormat="1" ht="16.5">
+    <row r="48" spans="1:20" s="69" customFormat="1" ht="14.95">
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -3789,7 +3803,7 @@
       <c r="S48" s="67"/>
       <c r="T48" s="67"/>
     </row>
-    <row r="49" spans="1:20" s="69" customFormat="1" ht="16.5">
+    <row r="49" spans="1:20" s="69" customFormat="1" ht="14.95">
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
@@ -3819,7 +3833,7 @@
       <c r="S49" s="67"/>
       <c r="T49" s="67"/>
     </row>
-    <row r="50" spans="1:20" s="69" customFormat="1" ht="115.5">
+    <row r="50" spans="1:20" s="69" customFormat="1" ht="119.55">
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -3853,7 +3867,7 @@
       <c r="S50" s="67"/>
       <c r="T50" s="67"/>
     </row>
-    <row r="51" spans="1:20" s="69" customFormat="1" ht="33">
+    <row r="51" spans="1:20" s="69" customFormat="1" ht="29.9">
       <c r="A51" s="22"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -3916,7 +3930,7 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="21.125" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
@@ -3930,7 +3944,7 @@
     <col min="13" max="13" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="27">
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="25.85">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -3995,7 +4009,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="47" customFormat="1" ht="27">
+    <row r="6" spans="1:14" s="47" customFormat="1" ht="25.85">
       <c r="A6" s="45" t="s">
         <v>63</v>
       </c>
@@ -4147,7 +4161,7 @@
       <c r="I16" s="53"/>
       <c r="J16" s="50"/>
     </row>
-    <row r="17" spans="1:1" ht="54">
+    <row r="17" spans="1:1" ht="51.65">
       <c r="A17" s="57" t="s">
         <v>72</v>
       </c>
@@ -4168,7 +4182,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="17.375" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.125" style="25" customWidth="1"/>
@@ -4182,7 +4196,7 @@
     <col min="13" max="16384" width="9" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" thickTop="1" thickBot="1">
+    <row r="1" spans="1:4" ht="19.05" thickTop="1" thickBot="1">
       <c r="A1" s="40"/>
       <c r="B1" s="39" t="s">
         <v>50</v>
@@ -4194,7 +4208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:4" ht="46.2" thickTop="1" thickBot="1">
       <c r="A2" s="26" t="s">
         <v>47</v>
       </c>
@@ -4206,7 +4220,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="1:4" ht="34.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:4" ht="28.55" thickTop="1" thickBot="1">
       <c r="A3" s="26" t="s">
         <v>44</v>
       </c>
@@ -4218,7 +4232,7 @@
       </c>
       <c r="D3" s="34"/>
     </row>
-    <row r="4" spans="1:4" ht="117" thickTop="1" thickBot="1">
+    <row r="4" spans="1:4" ht="106" thickTop="1" thickBot="1">
       <c r="A4" s="26" t="s">
         <v>42</v>
       </c>
@@ -4232,7 +4246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34.5" thickTop="1" thickBot="1">
+    <row r="5" spans="1:4" ht="28.55" thickTop="1" thickBot="1">
       <c r="A5" s="26" t="s">
         <v>38</v>
       </c>
@@ -4242,7 +4256,7 @@
       <c r="C5" s="28"/>
       <c r="D5" s="27"/>
     </row>
-    <row r="6" spans="1:4" ht="34.5" thickTop="1" thickBot="1">
+    <row r="6" spans="1:4" ht="42.15" thickTop="1" thickBot="1">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -4254,7 +4268,7 @@
       </c>
       <c r="D6" s="27"/>
     </row>
-    <row r="7" spans="1:4" ht="100.5" thickTop="1" thickBot="1">
+    <row r="7" spans="1:4" ht="82.9" thickTop="1" thickBot="1">
       <c r="A7" s="26" t="s">
         <v>34</v>
       </c>
@@ -4264,7 +4278,7 @@
       <c r="C7" s="28"/>
       <c r="D7" s="27"/>
     </row>
-    <row r="8" spans="1:4" ht="84" thickTop="1" thickBot="1">
+    <row r="8" spans="1:4" ht="76.099999999999994" thickTop="1" thickBot="1">
       <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
@@ -4274,7 +4288,7 @@
       <c r="C8" s="28"/>
       <c r="D8" s="32"/>
     </row>
-    <row r="9" spans="1:4" ht="84" thickTop="1" thickBot="1">
+    <row r="9" spans="1:4" ht="76.099999999999994" thickTop="1" thickBot="1">
       <c r="A9" s="26" t="s">
         <v>29</v>
       </c>
@@ -4286,7 +4300,7 @@
       </c>
       <c r="D9" s="27"/>
     </row>
-    <row r="10" spans="1:4" ht="249" thickTop="1" thickBot="1">
+    <row r="10" spans="1:4" ht="225.55" thickTop="1" thickBot="1">
       <c r="A10" s="26" t="s">
         <v>28</v>
       </c>
@@ -4298,7 +4312,7 @@
       </c>
       <c r="D10" s="27"/>
     </row>
-    <row r="11" spans="1:4" ht="18" thickTop="1" thickBot="1">
+    <row r="11" spans="1:4" ht="16.3" thickTop="1" thickBot="1">
       <c r="A11" s="31" t="s">
         <v>26</v>
       </c>
@@ -4308,7 +4322,7 @@
       <c r="C11" s="28"/>
       <c r="D11" s="27"/>
     </row>
-    <row r="12" spans="1:4" ht="18" thickTop="1" thickBot="1">
+    <row r="12" spans="1:4" ht="16.3" thickTop="1" thickBot="1">
       <c r="A12" s="31" t="s">
         <v>24</v>
       </c>
@@ -4318,7 +4332,7 @@
       <c r="C12" s="28"/>
       <c r="D12" s="27"/>
     </row>
-    <row r="13" spans="1:4" ht="133.5" thickTop="1" thickBot="1">
+    <row r="13" spans="1:4" ht="165.75" thickTop="1" thickBot="1">
       <c r="A13" s="26" t="s">
         <v>22</v>
       </c>
@@ -4330,7 +4344,7 @@
       </c>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="1:4" ht="18" thickTop="1" thickBot="1">
+    <row r="14" spans="1:4" ht="16.3" thickTop="1" thickBot="1">
       <c r="A14" s="30" t="s">
         <v>19</v>
       </c>
@@ -4340,7 +4354,7 @@
       <c r="C14" s="28"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:4" ht="14.25" thickTop="1"/>
+    <row r="15" spans="1:4" ht="13.6" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
@@ -4364,13 +4378,13 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="72.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="16.5">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="13.6">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
@@ -4381,7 +4395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="16.5">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="14.95">
       <c r="A2" s="10">
         <v>43278</v>
       </c>
@@ -4389,20 +4403,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.95">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="16.5">
+    <row r="4" spans="1:3" ht="14.95">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="16.5">
+    <row r="5" spans="1:3" ht="14.95">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
@@ -4457,7 +4471,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="29.375" customWidth="1"/>
@@ -4465,18 +4479,18 @@
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+    <row r="1" spans="1:4" ht="18.7" customHeight="1">
       <c r="A1" s="70" t="s">
         <v>180</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>